<commit_message>
Add tiled matrix mult and vectorized coarse mult, plus results
</commit_message>
<xml_diff>
--- a/data/NaiveMatrixMultVsCuBLAS_GFLOPS.xlsx
+++ b/data/NaiveMatrixMultVsCuBLAS_GFLOPS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malep\Documents\GitHub\CUDA-Playground\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DDA31B20-619A-48FF-90D5-BA78EC2BEC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB9EAE0-3FF5-4B5F-8756-7ED9EFFB24C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D0BAB987-745C-4FBC-B433-7BE29EB01B5E}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{D0BAB987-745C-4FBC-B433-7BE29EB01B5E}"/>
   </bookViews>
   <sheets>
     <sheet name="NaiveMatrixMultVsCuBLAS_GFLOPS" sheetId="1" r:id="rId1"/>
@@ -512,8 +512,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2165,24 +2168,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3272BF0A-F8FD-419F-A9DD-875B39EBE287}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>